<commit_message>
Set up CNS analysis
</commit_message>
<xml_diff>
--- a/02_output/bulk_density_mean.xlsx
+++ b/02_output/bulk_density_mean.xlsx
@@ -1,127 +1,150 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f304f79f068e311c/Universitaet/MASTER/MasterThesis/11_Data_Analysis_MA/02_output/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_B496D3386731ABD40AC42ABF073E1B9392599665" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CAAF5F7A-52B7-4275-A341-5E63875B6E9C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$B$33</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
-    <t xml:space="preserve">sample_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean(BD_g_cm3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1_1_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1_1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1_1_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2_1_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2_1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2_1_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2_2_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2_2_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3_1_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3_1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3_1_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3_2_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3_2_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3_2_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4_1_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4_1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4_1_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4_2_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4_2_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4_2_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5_1_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5_1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5_1_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5_2_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5_2_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5_2_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6_1_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6_1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6_1_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6_2_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6_2_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6_2_3</t>
+    <t>sample_name</t>
+  </si>
+  <si>
+    <t>mean(BD_g_cm3)</t>
+  </si>
+  <si>
+    <t>1_1_1</t>
+  </si>
+  <si>
+    <t>1_1_2</t>
+  </si>
+  <si>
+    <t>1_1_3</t>
+  </si>
+  <si>
+    <t>2_1_1</t>
+  </si>
+  <si>
+    <t>2_1_2</t>
+  </si>
+  <si>
+    <t>2_1_3</t>
+  </si>
+  <si>
+    <t>2_2_1</t>
+  </si>
+  <si>
+    <t>2_2_3</t>
+  </si>
+  <si>
+    <t>3_1_1</t>
+  </si>
+  <si>
+    <t>3_1_2</t>
+  </si>
+  <si>
+    <t>3_1_3</t>
+  </si>
+  <si>
+    <t>3_2_1</t>
+  </si>
+  <si>
+    <t>3_2_2</t>
+  </si>
+  <si>
+    <t>3_2_3</t>
+  </si>
+  <si>
+    <t>4_1_1</t>
+  </si>
+  <si>
+    <t>4_1_2</t>
+  </si>
+  <si>
+    <t>4_1_3</t>
+  </si>
+  <si>
+    <t>4_2_1</t>
+  </si>
+  <si>
+    <t>4_2_2</t>
+  </si>
+  <si>
+    <t>4_2_3</t>
+  </si>
+  <si>
+    <t>5_1_1</t>
+  </si>
+  <si>
+    <t>5_1_2</t>
+  </si>
+  <si>
+    <t>5_1_3</t>
+  </si>
+  <si>
+    <t>5_2_1</t>
+  </si>
+  <si>
+    <t>5_2_2</t>
+  </si>
+  <si>
+    <t>5_2_3</t>
+  </si>
+  <si>
+    <t>6_1_1</t>
+  </si>
+  <si>
+    <t>6_1_2</t>
+  </si>
+  <si>
+    <t>6_1_3</t>
+  </si>
+  <si>
+    <t>6_2_1</t>
+  </si>
+  <si>
+    <t>6_2_2</t>
+  </si>
+  <si>
+    <t>6_2_3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -154,9 +177,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -438,14 +470,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28:B30"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -453,264 +488,273 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" hidden="1" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="n">
-        <v>1.19272306481298</v>
-      </c>
-    </row>
-    <row r="3">
+      <c r="B2">
+        <v>1.1927230648129801</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="n">
-        <v>1.15094660843231</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="B3">
+        <v>1.1509466084323099</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="n">
-        <v>1.18204336919687</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="B4">
+        <v>1.1820433691968699</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="n">
-        <v>1.10592436220753</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="B5">
+        <v>1.1059243622075301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" hidden="1" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="n">
-        <v>1.35731602077892</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="B6">
+        <v>1.3573160207789201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" hidden="1" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>1.37323086130489</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:2" hidden="1" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>1.47751494790926</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="n">
-        <v>1.21581005386545</v>
-      </c>
-    </row>
-    <row r="10">
+      <c r="B9">
+        <v>1.2158100538654499</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="n">
-        <v>1.02786835160155</v>
-      </c>
-    </row>
-    <row r="11">
+      <c r="B10">
+        <v>1.0278683516015501</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>1.0073465835549</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:2" hidden="1" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" t="n">
-        <v>1.12037336215874</v>
-      </c>
-    </row>
-    <row r="13">
+      <c r="B12">
+        <v>1.1203733621587399</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13">
         <v>1.06022154714447</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14">
         <v>1.08728724632844</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>1.17026429314969</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:2" hidden="1" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>16</v>
       </c>
-      <c r="B16" t="n">
-        <v>1.19361303944765</v>
-      </c>
-    </row>
-    <row r="17">
+      <c r="B16">
+        <v>1.1936130394476501</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-      <c r="B17" t="n">
-        <v>1.23601771321751</v>
-      </c>
-    </row>
-    <row r="18">
+      <c r="B17">
+        <v>1.2360177132175101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>18</v>
       </c>
-      <c r="B18" t="n">
-        <v>1.17879757935276</v>
-      </c>
-    </row>
-    <row r="19">
+      <c r="B18">
+        <v>1.1787975793527601</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B19" t="n">
-        <v>1.24114815522917</v>
-      </c>
-    </row>
-    <row r="20">
+      <c r="B19">
+        <v>1.2411481552291701</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
         <v>20</v>
       </c>
-      <c r="B20" t="n">
-        <v>1.24303280739672</v>
-      </c>
-    </row>
-    <row r="21">
+      <c r="B20">
+        <v>1.2430328073967201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
         <v>21</v>
       </c>
-      <c r="B21" t="n">
-        <v>1.21858468066768</v>
-      </c>
-    </row>
-    <row r="22">
+      <c r="B21">
+        <v>1.2185846806676801</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
         <v>22</v>
       </c>
-      <c r="B22" t="n">
-        <v>1.20230337999802</v>
-      </c>
-    </row>
-    <row r="23">
+      <c r="B22">
+        <v>1.2023033799980201</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.75">
       <c r="A23" t="s">
         <v>23</v>
       </c>
-      <c r="B23" t="n">
-        <v>1.22391929333082</v>
-      </c>
-    </row>
-    <row r="24">
+      <c r="B23">
+        <v>1.2239192933308201</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.75">
       <c r="A24" t="s">
         <v>24</v>
       </c>
-      <c r="B24" t="n">
+      <c r="B24">
         <v>1.2067009017223</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.75">
       <c r="A25" t="s">
         <v>25</v>
       </c>
-      <c r="B25" t="n">
+      <c r="B25">
         <v>1.16089338376104</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.75">
       <c r="A26" t="s">
         <v>26</v>
       </c>
-      <c r="B26" t="n">
-        <v>1.21475255459366</v>
-      </c>
-    </row>
-    <row r="27">
+      <c r="B26">
+        <v>1.2147525545936599</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.75">
       <c r="A27" t="s">
         <v>27</v>
       </c>
-      <c r="B27" t="n">
+      <c r="B27">
         <v>1.16561548446973</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A28" t="s">
         <v>28</v>
       </c>
-      <c r="B28" t="n">
+      <c r="B28">
         <v>1.41165682494325</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A29" t="s">
         <v>29</v>
       </c>
-      <c r="B29" t="n">
-        <v>1.24093874943277</v>
-      </c>
-    </row>
-    <row r="30">
+      <c r="B29">
+        <v>1.2409387494327699</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A30" t="s">
         <v>30</v>
       </c>
-      <c r="B30" t="n">
+      <c r="B30">
         <v>1.05425348194723</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.75">
       <c r="A31" t="s">
         <v>31</v>
       </c>
-      <c r="B31" t="n">
-        <v>1.31208436875774</v>
-      </c>
-    </row>
-    <row r="32">
+      <c r="B31">
+        <v>1.3120843687577399</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.75">
       <c r="A32" t="s">
         <v>32</v>
       </c>
-      <c r="B32" t="n">
+      <c r="B32">
         <v>1.34302407517501</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.75">
       <c r="A33" t="s">
         <v>33</v>
       </c>
-      <c r="B33" t="n">
-        <v>1.29637893402817</v>
+      <c r="B33">
+        <v>1.2963789340281699</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B33" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="6_1_1"/>
+        <filter val="6_1_2"/>
+        <filter val="6_1_3"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>